<commit_message>
added works on final year project
</commit_message>
<xml_diff>
--- a/FinalYearDocuments/FYPYearSchedule.xlsx
+++ b/FinalYearDocuments/FYPYearSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FourthYearItems\GitRepoRetry\College_Y4\FinalYearDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3590A060-189B-4C35-8C0A-2D775D76D27C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C83CFF4-BBF3-4C1D-A9C4-F5F457950863}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{877ED0F0-078C-48B6-98B4-E7B144A1DE4F}"/>
   </bookViews>
@@ -628,10 +628,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EF1583-CE1F-4CB2-9C6E-4DD4F7274827}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,6 +1000,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>